<commit_message>
fix excel template cell remain old function
</commit_message>
<xml_diff>
--- a/quotation/files/inquiry_example_2.xlsx
+++ b/quotation/files/inquiry_example_2.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER 7\Documents\Python\Workspace\supplyChain\quotation\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A49BC96-5460-4AD4-B128-6E885010B148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A042C37C-446E-47B5-9061-FB042F1457B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A030683-3ABB-4E7A-BE27-3EEC33B51D3E}"/>
   </bookViews>
   <sheets>
     <sheet name="詢價單" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">詢價單!$A$1:$H$30</definedName>
   </definedNames>
@@ -463,6 +460,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,39 +531,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,58 +547,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="工作表1"/>
-      <sheetName val="模組"/>
-      <sheetName val="模組詢價單"/>
-      <sheetName val="電纜-伸泰"/>
-      <sheetName val="電纜詢價單-伸泰"/>
-      <sheetName val="電纜-大亞"/>
-      <sheetName val="電纜詢價單-大亞"/>
-      <sheetName val="電纜-台一"/>
-      <sheetName val="電纜詢價單-台一"/>
-      <sheetName val="歷史報價"/>
-      <sheetName val="逆變器-盛齊"/>
-      <sheetName val="逆變器詢價單-盛齊"/>
-      <sheetName val="逆變器詢價單-匯回"/>
-      <sheetName val="逆變器-協宸"/>
-      <sheetName val="逆變器詢價單-協宸"/>
-      <sheetName val="逆變器-菱台"/>
-      <sheetName val="逆變器詢價單-菱台"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="G2"/>
-        </row>
-        <row r="3">
-          <cell r="G3"/>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -907,7 +852,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:H5"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -922,96 +867,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" ht="33" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1043,14 +988,8 @@
       <c r="A9" s="6">
         <v>1</v>
       </c>
-      <c r="B9" s="6" t="str">
-        <f>IF(C9&lt;&gt;"","太陽能模組","")</f>
-        <v/>
-      </c>
-      <c r="C9" s="6" t="str">
-        <f>IF([1]模組!G2&lt;&gt;"",[1]模組!G2,"")</f>
-        <v/>
-      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="str">
         <f>IF(C9&lt;&gt;"",1,"")</f>
@@ -1064,17 +1003,11 @@
       <c r="A10" s="6">
         <v>2</v>
       </c>
-      <c r="B10" s="6" t="str">
-        <f t="shared" ref="B10:B18" si="0">IF(C10&lt;&gt;"","太陽能模組","")</f>
-        <v/>
-      </c>
-      <c r="C10" s="6" t="str">
-        <f>IF([1]模組!G3&lt;&gt;"",[1]模組!G3,"")</f>
-        <v/>
-      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="str">
-        <f t="shared" ref="E10:E18" si="1">IF(C10&lt;&gt;"",1,"")</f>
+        <f t="shared" ref="E10:E18" si="0">IF(C10&lt;&gt;"",1,"")</f>
         <v/>
       </c>
       <c r="F10" s="6"/>
@@ -1085,17 +1018,11 @@
       <c r="A11" s="6">
         <v>3</v>
       </c>
-      <c r="B11" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C11" s="6" t="str">
-        <f>IF([1]模組!G4&lt;&gt;"",[1]模組!G4,"")</f>
-        <v/>
-      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F11" s="6"/>
@@ -1106,17 +1033,11 @@
       <c r="A12" s="6">
         <v>4</v>
       </c>
-      <c r="B12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C12" s="6" t="str">
-        <f>IF([1]模組!G5&lt;&gt;"",[1]模組!G5,"")</f>
-        <v/>
-      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F12" s="6"/>
@@ -1127,17 +1048,11 @@
       <c r="A13" s="6">
         <v>5</v>
       </c>
-      <c r="B13" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C13" s="6" t="str">
-        <f>IF([1]模組!G6&lt;&gt;"",[1]模組!G6,"")</f>
-        <v/>
-      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F13" s="6"/>
@@ -1148,17 +1063,11 @@
       <c r="A14" s="6">
         <v>6</v>
       </c>
-      <c r="B14" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C14" s="6" t="str">
-        <f>IF([1]模組!G7&lt;&gt;"",[1]模組!G7,"")</f>
-        <v/>
-      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F14" s="6"/>
@@ -1169,17 +1078,11 @@
       <c r="A15" s="6">
         <v>7</v>
       </c>
-      <c r="B15" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C15" s="6" t="str">
-        <f>IF([1]模組!G8&lt;&gt;"",[1]模組!G8,"")</f>
-        <v/>
-      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F15" s="6"/>
@@ -1190,17 +1093,11 @@
       <c r="A16" s="6">
         <v>8</v>
       </c>
-      <c r="B16" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C16" s="6" t="str">
-        <f>IF([1]模組!G9&lt;&gt;"",[1]模組!G9,"")</f>
-        <v/>
-      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F16" s="6"/>
@@ -1211,17 +1108,11 @@
       <c r="A17" s="6">
         <v>9</v>
       </c>
-      <c r="B17" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C17" s="6" t="str">
-        <f>IF([1]模組!G10&lt;&gt;"",[1]模組!G10,"")</f>
-        <v/>
-      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F17" s="6"/>
@@ -1232,17 +1123,11 @@
       <c r="A18" s="6">
         <v>10</v>
       </c>
-      <c r="B18" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C18" s="6" t="str">
-        <f>IF([1]模組!G11&lt;&gt;"",[1]模組!G11,"")</f>
-        <v/>
-      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F18" s="6"/>
@@ -1250,16 +1135,16 @@
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="33" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1409,17 +1294,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="E5:H5"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="E4:H4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="E5:H5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>